<commit_message>
screenshot test case describe
</commit_message>
<xml_diff>
--- a/TestSteps/TestSteps describe.xlsx
+++ b/TestSteps/TestSteps describe.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wuia/Desktop/AppiumAutotest/TestSteps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A1A31F9-2AF7-6F49-B08A-0B081B26B571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1837E5CB-50B8-F64E-88AE-1F66932A3213}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" firstSheet="1" activeTab="10" xr2:uid="{17451AC4-B350-7841-B1A7-70E9EEFFBF30}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" firstSheet="2" activeTab="11" xr2:uid="{17451AC4-B350-7841-B1A7-70E9EEFFBF30}"/>
   </bookViews>
   <sheets>
     <sheet name="vLauncher_Wallpaper" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <sheet name="STB_stopwatch" sheetId="8" r:id="rId9"/>
     <sheet name="STB_timer" sheetId="9" r:id="rId10"/>
     <sheet name="STB_marker" sheetId="10" r:id="rId11"/>
+    <sheet name="STB_screenshot" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="208">
   <si>
     <t>Steps</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -818,6 +819,50 @@
   </si>
   <si>
     <t>compare location different</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>crop</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>full screen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>open Screenshot</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Crop button</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Full screen button</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>delete Pictures files</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Save button</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>count Pictures file to verify file is saved</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>close saving popup</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Close button</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>get current app to verify close function</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2154,8 +2199,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{267CF906-6932-6B40-98DB-C50CCC2C8902}">
   <dimension ref="A1:O46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G9" zoomScale="92" workbookViewId="0">
-      <selection activeCell="O26" sqref="O26"/>
+    <sheetView zoomScale="93" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22"/>
@@ -2970,6 +3015,324 @@
     <row r="46" spans="6:11">
       <c r="K46" s="2" t="s">
         <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{054E4CB2-FD59-494E-944F-8F5E813F3883}">
+  <dimension ref="A1:K30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="22"/>
+  <cols>
+    <col min="1" max="2" width="13.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.83203125" style="2"/>
+    <col min="5" max="5" width="19.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="2"/>
+    <col min="7" max="7" width="46.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" style="2"/>
+    <col min="9" max="9" width="19.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.83203125" style="2"/>
+    <col min="11" max="11" width="46" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="B2" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="J2" s="2">
+        <v>1</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="B3" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="F3" s="2">
+        <v>2</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="J3" s="2">
+        <v>2</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="B4" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="F4" s="2">
+        <v>3</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="J4" s="2">
+        <v>3</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="B5" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="F5" s="2">
+        <v>4</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="J5" s="2">
+        <v>4</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="F6" s="2">
+        <v>5</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="J6" s="2">
+        <v>5</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="F7" s="2">
+        <v>6</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="F8" s="2">
+        <v>7</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="F9" s="2">
+        <v>8</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="G10" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="E12" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="F12" s="2">
+        <v>1</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="F13" s="2">
+        <v>2</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="F14" s="2">
+        <v>3</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="F15" s="2">
+        <v>4</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="F16" s="2">
+        <v>5</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="17" spans="5:7">
+      <c r="F17" s="2">
+        <v>6</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="18" spans="5:7">
+      <c r="F18" s="2">
+        <v>7</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="19" spans="5:7">
+      <c r="F19" s="2">
+        <v>8</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="20" spans="5:7">
+      <c r="F20" s="2">
+        <v>9</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="5:7">
+      <c r="G21" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="5:7">
+      <c r="E23" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="F23" s="2">
+        <v>1</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="5:7">
+      <c r="F24" s="2">
+        <v>2</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="25" spans="5:7">
+      <c r="F25" s="2">
+        <v>3</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="26" spans="5:7">
+      <c r="F26" s="2">
+        <v>4</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="27" spans="5:7">
+      <c r="F27" s="2">
+        <v>5</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="28" spans="5:7">
+      <c r="F28" s="2">
+        <v>6</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="29" spans="5:7">
+      <c r="F29" s="2">
+        <v>7</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="30" spans="5:7">
+      <c r="F30" s="2">
+        <v>8</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
csv report structure, WallPaper test case
</commit_message>
<xml_diff>
--- a/TestSteps/TestSteps describe.xlsx
+++ b/TestSteps/TestSteps describe.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wuia/Desktop/AppiumAutotest/TestSteps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDD58642-E44D-5644-A2D5-76E6C04A6F21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6685AB2A-452C-694B-AA62-6F3805560812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" activeTab="4" xr2:uid="{17451AC4-B350-7841-B1A7-70E9EEFFBF30}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" xr2:uid="{17451AC4-B350-7841-B1A7-70E9EEFFBF30}"/>
   </bookViews>
   <sheets>
     <sheet name="vLauncher_Wallpaper" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="201">
   <si>
     <t>Steps</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1313,7 +1313,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{676EA4B8-998D-1542-982E-CCBA629695EF}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -3707,20 +3707,23 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB1E3124-FA28-6A4B-854D-651EBA37B2FB}">
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="61.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="43.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="57" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="55.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="22">
+    <row r="1" spans="1:11" ht="22">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3738,8 +3741,17 @@
       <c r="G1" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="22">
+      <c r="I1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="22">
       <c r="A2" s="2"/>
       <c r="B2" s="4" t="s">
         <v>26</v>
@@ -3755,8 +3767,17 @@
       <c r="G2" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="22">
+      <c r="I2" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="J2" s="2">
+        <v>1</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="22">
       <c r="A3" s="2"/>
       <c r="B3" s="4" t="s">
         <v>27</v>
@@ -3770,8 +3791,15 @@
       <c r="G3" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="22">
+      <c r="I3" s="2"/>
+      <c r="J3" s="2">
+        <v>2</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="22">
       <c r="A4" s="2"/>
       <c r="B4" s="4" t="s">
         <v>29</v>
@@ -3785,8 +3813,15 @@
       <c r="G4" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="22">
+      <c r="I4" s="2"/>
+      <c r="J4" s="2">
+        <v>3</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="22">
       <c r="A5" s="2"/>
       <c r="B5" s="4" t="s">
         <v>199</v>
@@ -3800,8 +3835,15 @@
       <c r="G5" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="22">
+      <c r="I5" s="2"/>
+      <c r="J5" s="2">
+        <v>4</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="22">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -3813,8 +3855,14 @@
       <c r="G6" s="5" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="22">
+      <c r="J6" s="2">
+        <v>5</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="22">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -3826,8 +3874,11 @@
       <c r="G7" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="22">
+      <c r="K7" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="22">
       <c r="A8" s="2"/>
       <c r="B8" s="5"/>
       <c r="C8" s="2"/>
@@ -3840,7 +3891,7 @@
       </c>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:9" ht="22">
+    <row r="9" spans="1:11" ht="22">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -3852,7 +3903,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="22">
+    <row r="10" spans="1:11" ht="22">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -3861,13 +3912,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="22">
+    <row r="11" spans="1:11" ht="22">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:9" ht="22">
+    <row r="12" spans="1:11" ht="22">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -3882,7 +3933,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="22">
+    <row r="13" spans="1:11" ht="22">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -3895,7 +3946,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="22">
+    <row r="14" spans="1:11" ht="22">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -3908,7 +3959,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="22">
+    <row r="15" spans="1:11" ht="22">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -3921,7 +3972,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="22">
+    <row r="16" spans="1:11" ht="22">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -4176,59 +4227,12 @@
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
-      <c r="E36" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="F36" s="2">
-        <v>1</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="37" spans="1:7" ht="22">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2">
-        <v>2</v>
-      </c>
-      <c r="G37" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="22">
-      <c r="E38" s="2"/>
-      <c r="F38" s="2">
-        <v>3</v>
-      </c>
-      <c r="G38" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="22">
-      <c r="E39" s="2"/>
-      <c r="F39" s="2">
-        <v>24</v>
-      </c>
-      <c r="G39" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="22">
-      <c r="F40" s="2">
-        <v>25</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="22">
-      <c r="G41" s="2" t="s">
-        <v>23</v>
-      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>